<commit_message>
vault backup: 2023-01-04 14:26:47
</commit_message>
<xml_diff>
--- a/assets/excursion-budget.xlsx
+++ b/assets/excursion-budget.xlsx
@@ -4,19 +4,19 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="6000" windowHeight="5710"/>
+    <workbookView activeTab="2" windowWidth="6000" windowHeight="5710"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Sheet_Title" localSheetId="0">"Sheet1"</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="0">"Sheet2"</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
-    <definedName name="_xlnm.Sheet_Title" localSheetId="1">"Sheet2"</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="1">"Sheet3"</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">#REF!</definedName>
-    <definedName name="_xlnm.Sheet_Title" localSheetId="2">"Sheet3"</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="2">"Sheet1"</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">#REF!</definedName>
   </definedNames>
   <calcPr calcMode="auto" iterate="1" iterateCount="100" iterateDelta="0.001"/>
@@ -84,13 +84,13 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="0" width="26.28413461538462" customWidth="1"/>
+    <col min="1" max="1" style="0" width="9.142307692307693"/>
     <col min="2" max="256" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData/>
@@ -138,18 +138,131 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView workbookViewId="0" tabSelected="1">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="0" width="9.142307692307693"/>
+    <col min="1" max="1" style="0" width="37.85486778846154" customWidth="1"/>
     <col min="2" max="256" style="0" width="9.142307692307693"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="13.5">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>single</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>2 person</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="13.5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Meet the sloths</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="13.5">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Fuerte Amador, Panama</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="13.5">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Manta, Ecuador</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="13.5">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Lima, Peru</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="13.5">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>San Martin, Peru (Nature preserve)</t>
+        </is>
+      </c>
+      <c r="B9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="13.5">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Santiago, Chile</t>
+        </is>
+      </c>
+      <c r="B10">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="13.5">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Puerto Montt, Chile (Falls &amp; Lake cruise)</t>
+        </is>
+      </c>
+      <c r="B11">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="13.5">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>(above) -- Patagonia nature</t>
+        </is>
+      </c>
+      <c r="B12">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="13.5">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Punta Arenas, Chile (penguine preserve)</t>
+        </is>
+      </c>
+      <c r="B13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="13.5">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Ushuaia, Arg. (train to end of world)</t>
+        </is>
+      </c>
+      <c r="B14">
+        <v>165</v>
+      </c>
+    </row>
+  </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <printOptions/>
   <pageMargins left="1" right="1" top="1.6666666666666667" bottom="1.6666666666666667" header="1" footer="1"/>

</xml_diff>

<commit_message>
vault backup: 2023-01-04 14:56:55
</commit_message>
<xml_diff>
--- a/assets/excursion-budget.xlsx
+++ b/assets/excursion-budget.xlsx
@@ -22,14 +22,6 @@
   <calcPr calcMode="auto" iterate="1" iterateCount="100" iterateDelta="0.001"/>
   <webPublishing allowPng="1" css="0" characterSet="UTF-8"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1" count="1">
-  <si>
-    <t>Total</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -169,16 +161,16 @@
   </sheetPr>
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0" tabSelected="1">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0" tabSelected="1">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="0" width="37.85486778846154" customWidth="1"/>
+    <col min="1" max="1" style="0" width="44.14020432692308" customWidth="1"/>
     <col min="2" max="2" style="0" width="13.570612980769232" customWidth="1"/>
     <col min="3" max="3" style="0" width="13.856310096153848" customWidth="1"/>
-    <col min="4" max="4" style="0" width="9.285156250000002" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" style="0" width="16.570432692307694" customWidth="1"/>
     <col min="5" max="256" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
@@ -202,15 +194,19 @@
     <row r="3" spans="1:4" ht="13.5">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Meet the sloths</t>
+          <t>Puerto Limon, Costa Rica (Cultural &amp; Soul food)</t>
         </is>
       </c>
       <c r="B3" s="1">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="C3" s="1">
         <f>B3*2</f>
-        <v>240</v>
+        <v>180</v>
+      </c>
+      <c r="D3" s="1">
+        <f>C3</f>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="13.5">
@@ -552,20 +548,22 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="13.5">
-      <c r="A27" s="2" t="s">
-        <v>0</v>
+      <c r="A27" s="2" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
       </c>
       <c r="B27" s="1">
         <f>SUM(B3:B26)</f>
-        <v>2934</v>
+        <v>2904</v>
       </c>
       <c r="C27" s="1">
         <f>SUM(C3:C26)</f>
-        <v>5868</v>
+        <v>5808</v>
       </c>
       <c r="D27" s="1">
         <f>SUM(D3:D26)</f>
-        <v>880</v>
+        <v>1060</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vault backup: 2023-01-21 08:10:43
</commit_message>
<xml_diff>
--- a/assets/excursion-budget.xlsx
+++ b/assets/excursion-budget.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="2" windowWidth="12000" windowHeight="5710"/>
+    <workbookView activeTab="2" windowWidth="21600" windowHeight="10450"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -111,8 +111,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="0" width="9.142307692307693"/>
-    <col min="2" max="256" style="0" width="9.142307692307693"/>
+    <col min="1" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData/>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
@@ -139,8 +138,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="0" width="9.142307692307693"/>
-    <col min="2" max="256" style="0" width="9.142307692307693"/>
+    <col min="1" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData/>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
@@ -162,19 +160,17 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="0" width="44.14020432692308" customWidth="1"/>
-    <col min="2" max="2" style="0" width="13.570612980769232" customWidth="1"/>
-    <col min="3" max="3" style="0" width="13.856310096153848" customWidth="1"/>
-    <col min="4" max="4" style="0" width="16.570432692307694" customWidth="1"/>
-    <col min="5" max="256" style="0" width="9.142307692307693"/>
+    <col min="1" max="1" style="0" width="73.99555288461539" customWidth="1"/>
+    <col min="2" max="4" style="0" width="20.284495192307695" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13.5">
+    <row r="1" spans="1:4" ht="22.5">
       <c r="B1" t="inlineStr">
         <is>
           <t>single</t>
@@ -191,7 +187,7 @@
         </is>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13.5">
+    <row r="3" spans="1:4" ht="22.5">
       <c r="A3" t="inlineStr">
         <is>
           <t>Puerto Limon, Costa Rica (Cultural &amp; Soul food)</t>
@@ -209,7 +205,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="13.5">
+    <row r="4" spans="1:4" ht="22.5">
       <c r="A4" t="inlineStr">
         <is>
           <t>Fuerte Amador, Panama (Old Capital)</t>
@@ -227,7 +223,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="13.5">
+    <row r="5" spans="1:4" ht="22.5">
       <c r="A5" t="inlineStr">
         <is>
           <t>Manta, Ecuador (Nature?)</t>
@@ -245,7 +241,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="13.5">
+    <row r="6" spans="1:4" ht="22.5">
       <c r="A6" t="inlineStr">
         <is>
           <t>Lima, Peru (Indigenous?)</t>
@@ -259,7 +255,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="13.5">
+    <row r="7" spans="1:4" ht="22.5">
       <c r="A7" t="inlineStr">
         <is>
           <t>San Martin, Peru (Nature preserve)</t>
@@ -277,7 +273,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="13.5">
+    <row r="8" spans="1:4" ht="22.5">
       <c r="A8" t="inlineStr">
         <is>
           <t>Santiago, Chile (best of Pablo Neruda)</t>
@@ -295,7 +291,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="13.5">
+    <row r="9" spans="1:4" ht="22.5">
       <c r="A9" t="inlineStr">
         <is>
           <t>Puerto Montt, Chile (Falls &amp; Lake cruise)</t>
@@ -309,7 +305,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="13.5">
+    <row r="10" spans="1:4" ht="22.5">
       <c r="A10" t="inlineStr">
         <is>
           <t>(above) -- Patagonia nature</t>
@@ -323,7 +319,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="13.5">
+    <row r="11" spans="1:4" ht="22.5">
       <c r="A11" t="inlineStr">
         <is>
           <t>Punta Arenas, Chile (penguine preserve)</t>
@@ -337,7 +333,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="13.5">
+    <row r="12" spans="1:4" ht="22.5">
       <c r="A12" t="inlineStr">
         <is>
           <t>Ushuaia, Arg. (train to end of world)</t>
@@ -351,7 +347,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="13.5">
+    <row r="13" spans="1:4" ht="22.5">
       <c r="A13" t="inlineStr">
         <is>
           <t>Falkland Is (Joe's penguins)</t>
@@ -365,7 +361,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="13.5">
+    <row r="14" spans="1:4" ht="22.5">
       <c r="A14" t="inlineStr">
         <is>
           <t>Puerto Madryn, Arg (penguin adventure)</t>
@@ -379,7 +375,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="13.5">
+    <row r="15" spans="1:4" ht="22.5">
       <c r="A15" t="inlineStr">
         <is>
           <t>Montevideo, Uruguay</t>
@@ -393,7 +389,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="13.5">
+    <row r="16" spans="1:4" ht="22.5">
       <c r="A16" t="inlineStr">
         <is>
           <t>Buenos Aires</t>
@@ -407,7 +403,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="13.5">
+    <row r="17" spans="1:4" ht="22.5">
       <c r="A17" t="inlineStr">
         <is>
           <t>Sao Paulo, Brazil</t>
@@ -421,7 +417,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="13.5">
+    <row r="18" spans="1:4" ht="22.5">
       <c r="A18" t="inlineStr">
         <is>
           <t>Rio de Janeiro (Christ the Redeemer)</t>
@@ -435,7 +431,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="13.5">
+    <row r="19" spans="1:4" ht="22.5">
       <c r="A19" t="inlineStr">
         <is>
           <t>Salvador da Bahia (museums)</t>
@@ -449,7 +445,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="13.5">
+    <row r="20" spans="1:4" ht="22.5">
       <c r="A20" t="inlineStr">
         <is>
           <t>Recife, Brazil (Jewish heritage)</t>
@@ -463,7 +459,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="13.5">
+    <row r="21" spans="1:4" ht="22.5">
       <c r="A21" t="inlineStr">
         <is>
           <t>Belem, Brazil (Art &amp; Culture)</t>
@@ -477,7 +473,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="13.5">
+    <row r="22" spans="1:4" ht="22.5">
       <c r="A22" t="inlineStr">
         <is>
           <t>Santarem, Brazil (Tapajos National Forest)</t>
@@ -491,7 +487,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="13.5">
+    <row r="23" spans="1:4" ht="22.5">
       <c r="A23" t="inlineStr">
         <is>
           <t>Manaus, Brazil (Cruise Amazon)</t>
@@ -505,7 +501,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="13.5">
+    <row r="24" spans="1:4" ht="22.5">
       <c r="A24" t="inlineStr">
         <is>
           <t>Barbados</t>
@@ -519,7 +515,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="13.5">
+    <row r="25" spans="1:4" ht="22.5">
       <c r="A25" t="inlineStr">
         <is>
           <t>Island Traditions</t>
@@ -533,7 +529,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="13.5">
+    <row r="26" spans="1:4" ht="22.5">
       <c r="A26" t="inlineStr">
         <is>
           <t>Puerto Rico</t>
@@ -547,7 +543,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="13.5">
+    <row r="27" spans="1:4" ht="22.5">
       <c r="A27" s="2" t="inlineStr">
         <is>
           <t>Total</t>

</xml_diff>